<commit_message>
changes for tc added sign up account and all
</commit_message>
<xml_diff>
--- a/src/main/java/com/edinarealty/qa/testdata/EdinaRealityDataTable.xlsx
+++ b/src/main/java/com/edinarealty/qa/testdata/EdinaRealityDataTable.xlsx
@@ -1,27 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johndang/eclipse_workspace/EdinaRealtyWeb_v2/src/main/java/com/edinarealty/qa/testdata/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1D7E6A-6291-2E42-A4E3-4DB811179963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5240" yWindow="1380" windowWidth="28100" windowHeight="13900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5235" yWindow="1380" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="5" r:id="rId1"/>
     <sheet name="Signup Local Account" sheetId="11" r:id="rId2"/>
-    <sheet name="Login" sheetId="7" r:id="rId3"/>
-    <sheet name="Saved Searches" sheetId="2" r:id="rId4"/>
-    <sheet name="Saved Properties" sheetId="6" r:id="rId5"/>
-    <sheet name="My Settings" sheetId="8" r:id="rId6"/>
+    <sheet name="VerifyBrokenImage" sheetId="15" r:id="rId3"/>
+    <sheet name="VerifyBrokenLinks" sheetId="14" r:id="rId4"/>
+    <sheet name="SignIn" sheetId="7" r:id="rId5"/>
+    <sheet name="Saved Searches" sheetId="2" r:id="rId6"/>
+    <sheet name="Saved Properties" sheetId="6" r:id="rId7"/>
+    <sheet name="My Settings" sheetId="8" r:id="rId8"/>
+    <sheet name="SalesHistoryAndTax" sheetId="12" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -30,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="165">
   <si>
     <t>Active</t>
   </si>
@@ -179,24 +176,9 @@
     <t>Minneapolis</t>
   </si>
   <si>
-    <t>Akatsukimember1!</t>
-  </si>
-  <si>
-    <t>Cynthia.Astralis@gmail.com</t>
-  </si>
-  <si>
     <t>Cynthia Ambrosia</t>
   </si>
   <si>
-    <t>$503,365</t>
-  </si>
-  <si>
-    <t>MLS# 6102437</t>
-  </si>
-  <si>
-    <t>12238 62nd Street NE Otsego, MN, 55301</t>
-  </si>
-  <si>
     <t>$451,995</t>
   </si>
   <si>
@@ -260,18 +242,12 @@
     <t>Taylor.Smith@gmail.com</t>
   </si>
   <si>
-    <t>Ambrosia</t>
-  </si>
-  <si>
     <t>Failure - 2022/02/12 21:16:23</t>
   </si>
   <si>
     <t>Success - 2022/02/12 21:16:24</t>
   </si>
   <si>
-    <t>Cynthia</t>
-  </si>
-  <si>
     <t>Multi-Factor Authentication</t>
   </si>
   <si>
@@ -287,12 +263,6 @@
     <t>Local Account</t>
   </si>
   <si>
-    <t>9378844148</t>
-  </si>
-  <si>
-    <t>Cynthia+22@artofqa.com</t>
-  </si>
-  <si>
     <t>Sign Out</t>
   </si>
   <si>
@@ -305,36 +275,9 @@
     <t>11313 Brookview Road Woodbury, MN, 55129</t>
   </si>
   <si>
-    <t>Cynthia+198@artofqa.com</t>
-  </si>
-  <si>
-    <t>Success - 2022/03/13 10:33:57</t>
-  </si>
-  <si>
     <t>good</t>
   </si>
   <si>
-    <t>Cynthia+197@artofqa.com</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Failure - 2022/03/21 15:57:05</t>
-  </si>
-  <si>
-    <t>Success - 2022/03/21 15:57:06</t>
-  </si>
-  <si>
-    <t>Success - 2022/03/21 15:58:55</t>
-  </si>
-  <si>
-    <t>Success - 2022/03/21 16:00:53</t>
-  </si>
-  <si>
-    <t>Success - 2022/03/21 16:02:22</t>
-  </si>
-  <si>
     <t>test@artofqa.com</t>
   </si>
   <si>
@@ -348,9 +291,6 @@
   </si>
   <si>
     <t>Signup Local  Account (MFA)</t>
-  </si>
-  <si>
-    <t>Signup Microsoft Account (MFA )</t>
   </si>
   <si>
     <t>Signup Google Account (MFA)</t>
@@ -484,12 +424,6 @@
     <t>gmail:</t>
   </si>
   <si>
-    <t>Success - 2022/03/23 23:32:53</t>
-  </si>
-  <si>
-    <t>Success - 2022/03/23 23:32:54</t>
-  </si>
-  <si>
     <t>Failure - 2022/03/23 23:35:22</t>
   </si>
   <si>
@@ -509,14 +443,164 @@
   </si>
   <si>
     <t>Success - 2022/03/23 23:36:33</t>
+  </si>
+  <si>
+    <t>SignIn Local Account (Non-MFA)</t>
+  </si>
+  <si>
+    <t>SignIn Local  Account (MFA)</t>
+  </si>
+  <si>
+    <t>SignIn Google Account (MFA)</t>
+  </si>
+  <si>
+    <t>SignIn Microsoft Account (MFA )</t>
+  </si>
+  <si>
+    <t>test+2Mfa@artofqa.com</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Tester2</t>
+  </si>
+  <si>
+    <t>NonMFA</t>
+  </si>
+  <si>
+    <t>Tester2 NonMFA</t>
+  </si>
+  <si>
+    <t>test+11@artofqa.com</t>
+  </si>
+  <si>
+    <t>Artofqa!123$</t>
+  </si>
+  <si>
+    <t>Tester20</t>
+  </si>
+  <si>
+    <t>NonMFA10</t>
+  </si>
+  <si>
+    <t>test+67@artofqa.com</t>
+  </si>
+  <si>
+    <t>7579193233</t>
+  </si>
+  <si>
+    <t>srm090@outlook.com</t>
+  </si>
+  <si>
+    <t>Tester110</t>
+  </si>
+  <si>
+    <t>NonMFA110</t>
+  </si>
+  <si>
+    <t>Tester110 NonMFA110</t>
+  </si>
+  <si>
+    <t>Success - 2022/04/01 18:57:04</t>
+  </si>
+  <si>
+    <t>Success - 2022/04/01 18:57:05</t>
+  </si>
+  <si>
+    <t>Success - 2022/04/01 18:59:28</t>
+  </si>
+  <si>
+    <t>Tester221</t>
+  </si>
+  <si>
+    <t>Tester221 NonMFA</t>
+  </si>
+  <si>
+    <t>BMcCjmpqKIwJvhX7I1WSTK--b8P1Rld7Vr4Q3Rai</t>
+  </si>
+  <si>
+    <t>Test123$</t>
+  </si>
+  <si>
+    <t>Signup Microsoft Account (Non-MFA )</t>
+  </si>
+  <si>
+    <t>Google requires valid phone number notaccepting twilio</t>
+  </si>
+  <si>
+    <t>create a microsoft account and update the userid column</t>
+  </si>
+  <si>
+    <t>test1 test1</t>
+  </si>
+  <si>
+    <t>PropertyState</t>
+  </si>
+  <si>
+    <t>PropertyNameValue</t>
+  </si>
+  <si>
+    <t>3041 Holmes Avenue S #201</t>
+  </si>
+  <si>
+    <t>Sales History and Tax Summary</t>
+  </si>
+  <si>
+    <t>6162224</t>
+  </si>
+  <si>
+    <t>Failure - 2022/04/07 19:06:23</t>
+  </si>
+  <si>
+    <t>Success - 2022/04/07 19:35:57</t>
+  </si>
+  <si>
+    <t>Success - 2022/04/07 19:35:59</t>
+  </si>
+  <si>
+    <t>Success - 2022/04/07 19:36:00</t>
+  </si>
+  <si>
+    <t>Verify Broken Links</t>
+  </si>
+  <si>
+    <t>Success - 2022/04/07 21:55:38</t>
+  </si>
+  <si>
+    <t>Verify Broken Image</t>
+  </si>
+  <si>
+    <t>Success - 2022/04/07 22:34:00</t>
+  </si>
+  <si>
+    <t>Failure - 2022/04/08 20:21:01</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Success - 2022/04/08 20:21:02</t>
+  </si>
+  <si>
+    <t>Success - 2022/04/08 20:21:03</t>
+  </si>
+  <si>
+    <t>Success - 2022/04/08 20:24:33</t>
+  </si>
+  <si>
+    <t>Failure - 2022/04/08 20:39:46</t>
+  </si>
+  <si>
+    <t>Failure - 2022/04/08 20:41:09</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -689,7 +773,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -724,7 +808,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -908,183 +992,192 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F10A5BE-02FF-4A02-B25D-58405473E643}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" style="6" width="8.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="6" width="15.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="6" width="30.33203125" collapsed="true"/>
-    <col min="4" max="16384" style="6" width="8.83203125" collapsed="true"/>
+    <col min="1" max="1" style="6" width="8.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="6" width="15.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="6" width="30.28515625" collapsed="true"/>
+    <col min="4" max="6" style="6" width="8.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="6" width="129.42578125" collapsed="true"/>
+    <col min="8" max="16384" style="6" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7">
       <c r="B2" s="6" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7">
       <c r="G3" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
       <c r="B4" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="C5" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="G6" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G6" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+      <c r="D7" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="C8" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:7">
       <c r="C9" s="9">
         <v>19378844148</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
       <c r="G11" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
       <c r="B12" s="6" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
       <c r="C13" s="6" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7">
       <c r="B16" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
       <c r="B17" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
       <c r="B18" s="10" t="s">
         <v>39</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
       <c r="B19" s="10" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
       <c r="B20" s="10" t="s">
         <v>40</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
       <c r="C21" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{14BB55BC-1571-EA47-9C53-EAC37A2296C9}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{12265120-0BA9-4247-B2C4-DCFD0FE475BC}"/>
-    <hyperlink ref="C12" r:id="rId3" xr:uid="{5DA04507-09F9-8144-96BA-F6A865C6CF3C}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C12" r:id="rId3"/>
+    <hyperlink ref="C7" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59DD63BA-0F5D-6243-AADD-DDAF84A76A87}">
-  <dimension ref="A1:N5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.1640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="28.1640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.5" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.1640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.1640625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.83203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="15.5" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.5" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="21.83203125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="7.5" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
     <col min="14" max="14" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1095,25 +1188,25 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="K1" t="s">
         <v>9</v>
@@ -1122,161 +1215,225 @@
         <v>8</v>
       </c>
       <c r="M1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="N1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
+        <v>122</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="I2" t="s">
         <v>7</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="K2" t="s">
         <v>10</v>
       </c>
       <c r="L2" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
       <c r="M2" t="s">
-        <v>7</v>
+        <v>120</v>
       </c>
       <c r="N2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="G3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H3" t="s">
-        <v>49</v>
+        <v>127</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="I3" t="s">
         <v>6</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>85</v>
+        <v>129</v>
       </c>
       <c r="K3" t="s">
         <v>10</v>
       </c>
       <c r="L3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M3" t="s">
-        <v>7</v>
+        <v>120</v>
       </c>
       <c r="N3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G4" t="s">
+        <v>122</v>
+      </c>
+      <c r="H4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" t="s">
+        <v>138</v>
+      </c>
+      <c r="M4" t="s">
+        <v>120</v>
+      </c>
+      <c r="N4" t="s">
+        <v>135</v>
+      </c>
+      <c r="P4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>109</v>
+        <v>90</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H5" t="s">
+        <v>125</v>
+      </c>
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" t="s">
+        <v>133</v>
+      </c>
+      <c r="M5" t="s">
+        <v>120</v>
+      </c>
+      <c r="N5" t="s">
+        <v>136</v>
+      </c>
+      <c r="P5" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{3CD868E4-0212-7A4D-8608-B15111BB0327}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{F857E5DE-4AFD-224B-AAA8-4F32DDCD6AA6}"/>
+    <hyperlink ref="C4" r:id="rId1"/>
+    <hyperlink ref="E4" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId4"/>
+    <hyperlink ref="E5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81561E1F-4A7A-402A-B47C-74A7286A6E6E}">
-  <dimension ref="A1:K6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.5" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="32.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.5" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="25.5" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="25.6640625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="20.33203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="7.5" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="9.83203125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1287,7 +1444,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1296,7 +1453,7 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
@@ -1305,172 +1462,338 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="K1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="1:11" s="11" customFormat="1">
+      <c r="A2" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="D2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>7</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" t="s">
-        <v>7</v>
+        <v>144</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="K2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="K5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>109</v>
-      </c>
-      <c r="K6" t="s">
-        <v>128</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{74BB9A84-4EFB-8747-B5EE-023F15C4C04F}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{8780D23B-1309-BE41-AD61-E2F657DECFA1}"/>
-    <hyperlink ref="E3" r:id="rId3" xr:uid="{A7E64F69-0E43-2749-8D41-E9251F3284BD}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843255FF-0F55-46C9-AC2A-3383A4362F23}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="11" customFormat="1">
+      <c r="A2" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>144</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="K2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:O3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="11" customFormat="1">
+      <c r="A2" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="K4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>90</v>
+      </c>
+      <c r="K5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="32.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.5" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="6" max="8" customWidth="true" width="21.5" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="18.5" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="27.5" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="6" max="8" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1505,7 +1828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1537,10 +1860,10 @@
         <v>47</v>
       </c>
       <c r="K2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1572,7 +1895,7 @@
         <v>48</v>
       </c>
       <c r="K3" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1580,38 +1903,38 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA4C4598-782C-4A85-A0C6-A7D664276002}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="32.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.5" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="6" max="8" customWidth="true" width="21.5" collapsed="true"/>
+    <col min="6" max="8" customWidth="true" width="21.42578125" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="18.5" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="18.42578125" collapsed="true"/>
     <col min="13" max="13" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="18.5" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="18.42578125" collapsed="true"/>
     <col min="17" max="17" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="18.5" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1676,7 +1999,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1705,43 +2028,43 @@
         <v>46</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>43</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>36</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="U2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1770,40 +2093,40 @@
         <v>36</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>46</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>43</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="U3" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1811,29 +2134,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{927D732F-D34E-4044-928A-9016C51E3FA3}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.1640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="28.1640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.1640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="27.1640625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="27.1640625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="9.83203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1841,103 +2164,218 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>62</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>63</v>
-      </c>
-      <c r="F1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" t="s">
-        <v>68</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" t="s">
         <v>72</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="J3" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{654953FF-934E-C347-88C2-5936DEACB386}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{E416F5E4-8E63-6143-952E-61ABBAEABCF3}"/>
-    <hyperlink ref="F3" r:id="rId3" xr:uid="{00EC34ED-C45D-B649-92D3-6751D086F176}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{0F5D83D8-C53C-E546-8025-B6D933D5844D}"/>
-    <hyperlink ref="I3" r:id="rId5" xr:uid="{9656114E-09AC-2A4A-BCAE-5ADB45860C0A}"/>
-    <hyperlink ref="I2" r:id="rId6" xr:uid="{0DD496F7-2A94-1347-BCB8-1FC42F843889}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="F3" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="I3" r:id="rId5"/>
+    <hyperlink ref="I2" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="11" max="12" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" t="s">
+        <v>145</v>
+      </c>
+      <c r="L1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>144</v>
+      </c>
+      <c r="J2" t="s">
+        <v>120</v>
+      </c>
+      <c r="K2" t="s">
+        <v>149</v>
+      </c>
+      <c r="L2" t="s">
+        <v>147</v>
+      </c>
+      <c r="M2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>